<commit_message>
Split the overlap of mass tolerances to prevent quant components being added to both lt and hv lists.
</commit_message>
<xml_diff>
--- a/Examples/proteoform_quantification_minimal_test.xlsx
+++ b/Examples/proteoform_quantification_minimal_test.xlsx
@@ -9788,15 +9788,15 @@
       </c>
       <c r="Q2">
         <f>N2-$U$3</f>
-        <v>-4.1437477202333337</v>
+        <v>-3.6437477202333333</v>
       </c>
       <c r="R2">
         <f>N2+$U$3</f>
-        <v>-2.1437477202333333</v>
+        <v>-2.6437477202333333</v>
       </c>
       <c r="S2" t="b">
-        <f>OR(O2&lt;Q2,O2&gt;R2)</f>
-        <v>1</v>
+        <f>OR(AND(O2&lt;Q2,O2&lt;0),AND(O2&gt;R2,O2&gt;0))</f>
+        <v>0</v>
       </c>
       <c r="U2" s="2">
         <v>1</v>
@@ -9871,18 +9871,18 @@
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q66" si="1">N3-$U$3</f>
-        <v>-2.2110134193333333</v>
+        <v>-1.7110134193333333</v>
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R66" si="2">N3+$U$3</f>
-        <v>-0.21101341933333329</v>
+        <v>-0.71101341933333329</v>
       </c>
       <c r="S3" t="b">
-        <f t="shared" ref="S3:S66" si="3">OR(O3&lt;Q3,O3&gt;R3)</f>
+        <f t="shared" ref="S3:S66" si="3">OR(AND(O3&lt;Q3,O3&lt;0),AND(O3&gt;R3,O3&gt;0))</f>
         <v>0</v>
       </c>
       <c r="U3" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="V3" s="11" t="s">
         <v>123</v>
@@ -9954,11 +9954,11 @@
       </c>
       <c r="Q4">
         <f t="shared" si="1"/>
-        <v>-1.8428559718333335</v>
+        <v>-1.3428559718333335</v>
       </c>
       <c r="R4">
         <f t="shared" si="2"/>
-        <v>0.15714402816666662</v>
+        <v>-0.34285597183333338</v>
       </c>
       <c r="S4" t="b">
         <f t="shared" si="3"/>
@@ -10037,15 +10037,15 @@
       </c>
       <c r="Q5">
         <f t="shared" si="1"/>
-        <v>-1.6885465138333333</v>
+        <v>-1.1885465138333333</v>
       </c>
       <c r="R5">
         <f t="shared" si="2"/>
-        <v>0.31145348616666668</v>
+        <v>-0.18854651383333332</v>
       </c>
       <c r="S5" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -10114,15 +10114,15 @@
       </c>
       <c r="Q6">
         <f t="shared" si="1"/>
-        <v>-1.6762810648333333</v>
+        <v>-1.1762810648333333</v>
       </c>
       <c r="R6">
         <f t="shared" si="2"/>
-        <v>0.32371893516666661</v>
+        <v>-0.17628106483333339</v>
       </c>
       <c r="S6" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -10191,15 +10191,15 @@
       </c>
       <c r="Q7">
         <f t="shared" si="1"/>
-        <v>-1.5512089903666668</v>
+        <v>-1.0512089903666668</v>
       </c>
       <c r="R7">
         <f t="shared" si="2"/>
-        <v>0.44879100963333329</v>
+        <v>-5.1208990366666707E-2</v>
       </c>
       <c r="S7" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -10268,15 +10268,15 @@
       </c>
       <c r="Q8">
         <f t="shared" si="1"/>
-        <v>-1.5112557897333332</v>
+        <v>-1.0112557897333332</v>
       </c>
       <c r="R8">
         <f t="shared" si="2"/>
-        <v>0.4887442102666667</v>
+        <v>-1.1255789733333299E-2</v>
       </c>
       <c r="S8" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -10345,15 +10345,15 @@
       </c>
       <c r="Q9">
         <f t="shared" si="1"/>
-        <v>-1.4783715209666666</v>
+        <v>-0.97837152096666657</v>
       </c>
       <c r="R9">
         <f t="shared" si="2"/>
-        <v>0.52162847903333343</v>
+        <v>2.162847903333337E-2</v>
       </c>
       <c r="S9" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -10422,18 +10422,18 @@
       </c>
       <c r="Q10">
         <f t="shared" si="1"/>
-        <v>-1.4550825898666666</v>
+        <v>-0.95508258986666661</v>
       </c>
       <c r="R10">
         <f t="shared" si="2"/>
-        <v>0.54491741013333339</v>
+        <v>4.4917410133333335E-2</v>
       </c>
       <c r="S10" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U10">
-        <v>-0.92235255849999997</v>
+        <v>-1000000</v>
       </c>
       <c r="V10" s="11" t="s">
         <v>126</v>
@@ -10505,18 +10505,18 @@
       </c>
       <c r="Q11">
         <f t="shared" si="1"/>
-        <v>-1.4162208630999999</v>
+        <v>-0.91622086309999995</v>
       </c>
       <c r="R11">
         <f t="shared" si="2"/>
-        <v>0.58377913690000005</v>
+        <v>8.3779136899999995E-2</v>
       </c>
       <c r="S11" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" s="2">
-        <v>5.9232634213999997</v>
+        <v>5.7716125598000003</v>
       </c>
       <c r="V11" s="11" t="s">
         <v>127</v>
@@ -10588,11 +10588,11 @@
       </c>
       <c r="Q12">
         <f t="shared" si="1"/>
-        <v>-1.4055734019333332</v>
+        <v>-0.90557340193333324</v>
       </c>
       <c r="R12">
         <f t="shared" si="2"/>
-        <v>0.59442659806666676</v>
+        <v>9.44265980666667E-2</v>
       </c>
       <c r="S12" t="b">
         <f t="shared" si="3"/>
@@ -10665,11 +10665,11 @@
       </c>
       <c r="Q13">
         <f t="shared" si="1"/>
-        <v>-1.3830229418</v>
+        <v>-0.88302294179999996</v>
       </c>
       <c r="R13">
         <f t="shared" si="2"/>
-        <v>0.61697705820000004</v>
+        <v>0.11697705819999998</v>
       </c>
       <c r="S13" t="b">
         <f t="shared" si="3"/>
@@ -10743,11 +10743,11 @@
       </c>
       <c r="Q14">
         <f t="shared" si="1"/>
-        <v>-1.3758152067</v>
+        <v>-0.87581520670000002</v>
       </c>
       <c r="R14">
         <f t="shared" si="2"/>
-        <v>0.62418479329999998</v>
+        <v>0.12418479329999998</v>
       </c>
       <c r="S14" t="b">
         <f t="shared" si="3"/>
@@ -10755,7 +10755,7 @@
       </c>
       <c r="U14" s="13">
         <f>COUNTIF(O:O,"&lt;="&amp;U10)+COUNTIF(O:O,"&gt;="&amp;U11)</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V14" s="2" t="s">
         <v>118</v>
@@ -10827,11 +10827,11 @@
       </c>
       <c r="Q15">
         <f t="shared" si="1"/>
-        <v>-1.3247319986666666</v>
+        <v>-0.82473199866666658</v>
       </c>
       <c r="R15">
         <f t="shared" si="2"/>
-        <v>0.67526800133333342</v>
+        <v>0.17526800133333337</v>
       </c>
       <c r="S15" t="b">
         <f t="shared" si="3"/>
@@ -10839,7 +10839,7 @@
       </c>
       <c r="U15" s="13">
         <f>(COUNTIFS(Sheet1!K:K,"&lt;"&amp;U10,Sheet1!K:K,"&lt;=0")+COUNTIFS(Sheet1!K:K,"&gt;"&amp;U11,Sheet1!K:K,"&gt;=0")+COUNTIFS(Sheet5!K:K,"&lt;"&amp;U10,Sheet5!K:K,"&lt;=0")+COUNTIFS(Sheet5!K:K,"&gt;"&amp;U11,Sheet5!K:K,"&gt;=0")+COUNTIFS(Sheet9!K:K,"&lt;"&amp;U10,Sheet9!K:K,"&lt;=0")+COUNTIFS(Sheet9!K:K,"&gt;"&amp;U11,Sheet9!K:K,"&gt;=0"))/3</f>
-        <v>2.3333333333333335</v>
+        <v>0</v>
       </c>
       <c r="V15" s="2" t="s">
         <v>119</v>
@@ -10911,11 +10911,11 @@
       </c>
       <c r="Q16">
         <f t="shared" si="1"/>
-        <v>-1.3117167717666667</v>
+        <v>-0.81171677176666668</v>
       </c>
       <c r="R16">
         <f t="shared" si="2"/>
-        <v>0.68828322823333332</v>
+        <v>0.18828322823333332</v>
       </c>
       <c r="S16" t="b">
         <f t="shared" si="3"/>
@@ -10989,11 +10989,11 @@
       </c>
       <c r="Q17">
         <f t="shared" si="1"/>
-        <v>-1.3061930973666667</v>
+        <v>-0.80619309736666667</v>
       </c>
       <c r="R17">
         <f t="shared" si="2"/>
-        <v>0.69380690263333333</v>
+        <v>0.19380690263333333</v>
       </c>
       <c r="S17" t="b">
         <f t="shared" si="3"/>
@@ -11001,7 +11001,7 @@
       </c>
       <c r="U17" s="13">
         <f>U15/U14</f>
-        <v>0.23333333333333334</v>
+        <v>0</v>
       </c>
       <c r="V17" s="2" t="s">
         <v>120</v>
@@ -11073,11 +11073,11 @@
       </c>
       <c r="Q18">
         <f t="shared" si="1"/>
-        <v>-1.2884567932666666</v>
+        <v>-0.78845679326666662</v>
       </c>
       <c r="R18">
         <f t="shared" si="2"/>
-        <v>0.71154320673333338</v>
+        <v>0.21154320673333332</v>
       </c>
       <c r="S18" t="b">
         <f t="shared" si="3"/>
@@ -11150,11 +11150,11 @@
       </c>
       <c r="Q19">
         <f t="shared" si="1"/>
-        <v>-1.2799935573333334</v>
+        <v>-0.77999355733333342</v>
       </c>
       <c r="R19">
         <f t="shared" si="2"/>
-        <v>0.72000644266666658</v>
+        <v>0.22000644266666664</v>
       </c>
       <c r="S19" t="b">
         <f t="shared" si="3"/>
@@ -11227,11 +11227,11 @@
       </c>
       <c r="Q20">
         <f t="shared" si="1"/>
-        <v>-1.2679772715666666</v>
+        <v>-0.76797727156666662</v>
       </c>
       <c r="R20">
         <f t="shared" si="2"/>
-        <v>0.73202272843333338</v>
+        <v>0.23202272843333333</v>
       </c>
       <c r="S20" t="b">
         <f t="shared" si="3"/>
@@ -11304,11 +11304,11 @@
       </c>
       <c r="Q21">
         <f t="shared" si="1"/>
-        <v>-1.2573809425333333</v>
+        <v>-0.75738094253333332</v>
       </c>
       <c r="R21">
         <f t="shared" si="2"/>
-        <v>0.74261905746666668</v>
+        <v>0.24261905746666668</v>
       </c>
       <c r="S21" t="b">
         <f t="shared" si="3"/>
@@ -11381,11 +11381,11 @@
       </c>
       <c r="Q22">
         <f t="shared" si="1"/>
-        <v>-1.2542734514333334</v>
+        <v>-0.75427345143333335</v>
       </c>
       <c r="R22">
         <f t="shared" si="2"/>
-        <v>0.74572654856666665</v>
+        <v>0.24572654856666665</v>
       </c>
       <c r="S22" t="b">
         <f t="shared" si="3"/>
@@ -11458,11 +11458,11 @@
       </c>
       <c r="Q23">
         <f t="shared" si="1"/>
-        <v>-1.2446293516666667</v>
+        <v>-0.74462935166666666</v>
       </c>
       <c r="R23">
         <f t="shared" si="2"/>
-        <v>0.75537064833333334</v>
+        <v>0.25537064833333334</v>
       </c>
       <c r="S23" t="b">
         <f t="shared" si="3"/>
@@ -11535,11 +11535,11 @@
       </c>
       <c r="Q24">
         <f t="shared" si="1"/>
-        <v>-1.2285446082333333</v>
+        <v>-0.72854460823333334</v>
       </c>
       <c r="R24">
         <f t="shared" si="2"/>
-        <v>0.77145539176666666</v>
+        <v>0.27145539176666666</v>
       </c>
       <c r="S24" t="b">
         <f t="shared" si="3"/>
@@ -11612,11 +11612,11 @@
       </c>
       <c r="Q25">
         <f t="shared" si="1"/>
-        <v>-1.2231548915000001</v>
+        <v>-0.72315489150000001</v>
       </c>
       <c r="R25">
         <f t="shared" si="2"/>
-        <v>0.77684510849999999</v>
+        <v>0.27684510849999999</v>
       </c>
       <c r="S25" t="b">
         <f t="shared" si="3"/>
@@ -11689,11 +11689,11 @@
       </c>
       <c r="Q26">
         <f t="shared" si="1"/>
-        <v>-1.2074028830666668</v>
+        <v>-0.70740288306666665</v>
       </c>
       <c r="R26">
         <f t="shared" si="2"/>
-        <v>0.79259711693333335</v>
+        <v>0.29259711693333335</v>
       </c>
       <c r="S26" t="b">
         <f t="shared" si="3"/>
@@ -11766,11 +11766,11 @@
       </c>
       <c r="Q27">
         <f t="shared" si="1"/>
-        <v>-1.1971384006333334</v>
+        <v>-0.69713840063333332</v>
       </c>
       <c r="R27">
         <f t="shared" si="2"/>
-        <v>0.80286159936666668</v>
+        <v>0.30286159936666668</v>
       </c>
       <c r="S27" t="b">
         <f t="shared" si="3"/>
@@ -11843,11 +11843,11 @@
       </c>
       <c r="Q28">
         <f t="shared" si="1"/>
-        <v>-1.1682461966</v>
+        <v>-0.66824619659999995</v>
       </c>
       <c r="R28">
         <f t="shared" si="2"/>
-        <v>0.83175380340000005</v>
+        <v>0.33175380340000005</v>
       </c>
       <c r="S28" t="b">
         <f t="shared" si="3"/>
@@ -11920,11 +11920,11 @@
       </c>
       <c r="Q29">
         <f t="shared" si="1"/>
-        <v>-1.1644694070333332</v>
+        <v>-0.66446940703333335</v>
       </c>
       <c r="R29">
         <f t="shared" si="2"/>
-        <v>0.83553059296666665</v>
+        <v>0.33553059296666665</v>
       </c>
       <c r="S29" t="b">
         <f t="shared" si="3"/>
@@ -11997,11 +11997,11 @@
       </c>
       <c r="Q30">
         <f t="shared" si="1"/>
-        <v>-1.1326123987000001</v>
+        <v>-0.63261239869999997</v>
       </c>
       <c r="R30">
         <f t="shared" si="2"/>
-        <v>0.86738760130000003</v>
+        <v>0.36738760130000003</v>
       </c>
       <c r="S30" t="b">
         <f t="shared" si="3"/>
@@ -12074,11 +12074,11 @@
       </c>
       <c r="Q31">
         <f t="shared" si="1"/>
-        <v>-1.1231358488666667</v>
+        <v>-0.62313584886666662</v>
       </c>
       <c r="R31">
         <f t="shared" si="2"/>
-        <v>0.87686415113333338</v>
+        <v>0.37686415113333332</v>
       </c>
       <c r="S31" t="b">
         <f t="shared" si="3"/>
@@ -12151,11 +12151,11 @@
       </c>
       <c r="Q32">
         <f t="shared" si="1"/>
-        <v>-1.1211152696333333</v>
+        <v>-0.6211152696333333</v>
       </c>
       <c r="R32">
         <f t="shared" si="2"/>
-        <v>0.8788847303666667</v>
+        <v>0.37888473036666664</v>
       </c>
       <c r="S32" t="b">
         <f t="shared" si="3"/>
@@ -12228,11 +12228,11 @@
       </c>
       <c r="Q33">
         <f t="shared" si="1"/>
-        <v>-1.1182965698333334</v>
+        <v>-0.61829656983333336</v>
       </c>
       <c r="R33">
         <f t="shared" si="2"/>
-        <v>0.88170343016666664</v>
+        <v>0.38170343016666669</v>
       </c>
       <c r="S33" t="b">
         <f t="shared" si="3"/>
@@ -12305,11 +12305,11 @@
       </c>
       <c r="Q34">
         <f t="shared" si="1"/>
-        <v>-1.1072695939333332</v>
+        <v>-0.60726959393333335</v>
       </c>
       <c r="R34">
         <f t="shared" si="2"/>
-        <v>0.89273040606666665</v>
+        <v>0.3927304060666667</v>
       </c>
       <c r="S34" t="b">
         <f t="shared" si="3"/>
@@ -12382,11 +12382,11 @@
       </c>
       <c r="Q35">
         <f t="shared" si="1"/>
-        <v>-1.1024462077999999</v>
+        <v>-0.60244620780000002</v>
       </c>
       <c r="R35">
         <f t="shared" si="2"/>
-        <v>0.89755379219999998</v>
+        <v>0.39755379219999998</v>
       </c>
       <c r="S35" t="b">
         <f t="shared" si="3"/>
@@ -12459,11 +12459,11 @@
       </c>
       <c r="Q36">
         <f t="shared" si="1"/>
-        <v>-1.0958970734</v>
+        <v>-0.59589707339999998</v>
       </c>
       <c r="R36">
         <f t="shared" si="2"/>
-        <v>0.90410292660000002</v>
+        <v>0.40410292660000002</v>
       </c>
       <c r="S36" t="b">
         <f t="shared" si="3"/>
@@ -12536,11 +12536,11 @@
       </c>
       <c r="Q37">
         <f t="shared" si="1"/>
-        <v>-1.0868000028</v>
+        <v>-0.5868000028</v>
       </c>
       <c r="R37">
         <f t="shared" si="2"/>
-        <v>0.9131999972</v>
+        <v>0.4131999972</v>
       </c>
       <c r="S37" t="b">
         <f t="shared" si="3"/>
@@ -12613,11 +12613,11 @@
       </c>
       <c r="Q38">
         <f t="shared" si="1"/>
-        <v>-1.0847795558666666</v>
+        <v>-0.58477955586666663</v>
       </c>
       <c r="R38">
         <f t="shared" si="2"/>
-        <v>0.91522044413333337</v>
+        <v>0.41522044413333331</v>
       </c>
       <c r="S38" t="b">
         <f t="shared" si="3"/>
@@ -12690,11 +12690,11 @@
       </c>
       <c r="Q39">
         <f t="shared" si="1"/>
-        <v>-1.0695987859666667</v>
+        <v>-0.56959878596666669</v>
       </c>
       <c r="R39">
         <f t="shared" si="2"/>
-        <v>0.93040121403333331</v>
+        <v>0.43040121403333331</v>
       </c>
       <c r="S39" t="b">
         <f t="shared" si="3"/>
@@ -12767,11 +12767,11 @@
       </c>
       <c r="Q40">
         <f t="shared" si="1"/>
-        <v>-1.0650993625666667</v>
+        <v>-0.56509936256666671</v>
       </c>
       <c r="R40">
         <f t="shared" si="2"/>
-        <v>0.93490063743333329</v>
+        <v>0.43490063743333335</v>
       </c>
       <c r="S40" t="b">
         <f t="shared" si="3"/>
@@ -12844,11 +12844,11 @@
       </c>
       <c r="Q41">
         <f t="shared" si="1"/>
-        <v>-1.0614610091333334</v>
+        <v>-0.5614610091333333</v>
       </c>
       <c r="R41">
         <f t="shared" si="2"/>
-        <v>0.9385389908666667</v>
+        <v>0.43853899086666664</v>
       </c>
       <c r="S41" t="b">
         <f t="shared" si="3"/>
@@ -12921,11 +12921,11 @@
       </c>
       <c r="Q42">
         <f t="shared" si="1"/>
-        <v>-1.0580776062333332</v>
+        <v>-0.55807760623333336</v>
       </c>
       <c r="R42">
         <f t="shared" si="2"/>
-        <v>0.94192239376666664</v>
+        <v>0.44192239376666664</v>
       </c>
       <c r="S42" t="b">
         <f t="shared" si="3"/>
@@ -12998,11 +12998,11 @@
       </c>
       <c r="Q43">
         <f t="shared" si="1"/>
-        <v>-1.0477572897333334</v>
+        <v>-0.54775728973333337</v>
       </c>
       <c r="R43">
         <f t="shared" si="2"/>
-        <v>0.95224271026666663</v>
+        <v>0.45224271026666668</v>
       </c>
       <c r="S43" t="b">
         <f t="shared" si="3"/>
@@ -13075,11 +13075,11 @@
       </c>
       <c r="Q44">
         <f t="shared" si="1"/>
-        <v>-1.0435373620333332</v>
+        <v>-0.54353736203333336</v>
       </c>
       <c r="R44">
         <f t="shared" si="2"/>
-        <v>0.95646263796666664</v>
+        <v>0.45646263796666664</v>
       </c>
       <c r="S44" t="b">
         <f t="shared" si="3"/>
@@ -13152,11 +13152,11 @@
       </c>
       <c r="Q45">
         <f t="shared" si="1"/>
-        <v>-1.0392732605333332</v>
+        <v>-0.53927326053333335</v>
       </c>
       <c r="R45">
         <f t="shared" si="2"/>
-        <v>0.96072673946666665</v>
+        <v>0.46072673946666665</v>
       </c>
       <c r="S45" t="b">
         <f t="shared" si="3"/>
@@ -13229,11 +13229,11 @@
       </c>
       <c r="Q46">
         <f t="shared" si="1"/>
-        <v>-1.0377450919</v>
+        <v>-0.53774509189999997</v>
       </c>
       <c r="R46">
         <f t="shared" si="2"/>
-        <v>0.96225490810000003</v>
+        <v>0.46225490810000003</v>
       </c>
       <c r="S46" t="b">
         <f t="shared" si="3"/>
@@ -13306,11 +13306,11 @@
       </c>
       <c r="Q47">
         <f t="shared" si="1"/>
-        <v>-1.0360063652</v>
+        <v>-0.5360063652</v>
       </c>
       <c r="R47">
         <f t="shared" si="2"/>
-        <v>0.9639936348</v>
+        <v>0.4639936348</v>
       </c>
       <c r="S47" t="b">
         <f t="shared" si="3"/>
@@ -13383,11 +13383,11 @@
       </c>
       <c r="Q48">
         <f t="shared" si="1"/>
-        <v>-1.0330002451</v>
+        <v>-0.53300024509999999</v>
       </c>
       <c r="R48">
         <f t="shared" si="2"/>
-        <v>0.96699975490000001</v>
+        <v>0.46699975490000001</v>
       </c>
       <c r="S48" t="b">
         <f t="shared" si="3"/>
@@ -13460,11 +13460,11 @@
       </c>
       <c r="Q49">
         <f t="shared" si="1"/>
-        <v>-1.0319995486</v>
+        <v>-0.53199954859999998</v>
       </c>
       <c r="R49">
         <f t="shared" si="2"/>
-        <v>0.96800045140000002</v>
+        <v>0.46800045140000002</v>
       </c>
       <c r="S49" t="b">
         <f t="shared" si="3"/>
@@ -13537,11 +13537,11 @@
       </c>
       <c r="Q50">
         <f t="shared" si="1"/>
-        <v>-1.0310430249</v>
+        <v>-0.53104302489999999</v>
       </c>
       <c r="R50">
         <f t="shared" si="2"/>
-        <v>0.96895697510000001</v>
+        <v>0.46895697510000001</v>
       </c>
       <c r="S50" t="b">
         <f t="shared" si="3"/>
@@ -13614,11 +13614,11 @@
       </c>
       <c r="Q51">
         <f t="shared" si="1"/>
-        <v>-1.0267392986999999</v>
+        <v>-0.52673929870000002</v>
       </c>
       <c r="R51">
         <f t="shared" si="2"/>
-        <v>0.97326070129999998</v>
+        <v>0.47326070129999998</v>
       </c>
       <c r="S51" t="b">
         <f t="shared" si="3"/>
@@ -13691,11 +13691,11 @@
       </c>
       <c r="Q52">
         <f t="shared" si="1"/>
-        <v>-1.0235752679000001</v>
+        <v>-0.52357526789999997</v>
       </c>
       <c r="R52">
         <f t="shared" si="2"/>
-        <v>0.97642473210000003</v>
+        <v>0.47642473210000003</v>
       </c>
       <c r="S52" t="b">
         <f t="shared" si="3"/>
@@ -13768,11 +13768,11 @@
       </c>
       <c r="Q53">
         <f t="shared" si="1"/>
-        <v>-1.0202178855999999</v>
+        <v>-0.52021788560000004</v>
       </c>
       <c r="R53">
         <f t="shared" si="2"/>
-        <v>0.97978211439999996</v>
+        <v>0.47978211440000001</v>
       </c>
       <c r="S53" t="b">
         <f t="shared" si="3"/>
@@ -13845,11 +13845,11 @@
       </c>
       <c r="Q54">
         <f t="shared" si="1"/>
-        <v>-1.0161025524666667</v>
+        <v>-0.5161025524666667</v>
       </c>
       <c r="R54">
         <f t="shared" si="2"/>
-        <v>0.9838974475333333</v>
+        <v>0.48389744753333336</v>
       </c>
       <c r="S54" t="b">
         <f t="shared" si="3"/>
@@ -13922,11 +13922,11 @@
       </c>
       <c r="Q55">
         <f t="shared" si="1"/>
-        <v>-1.0094677783999999</v>
+        <v>-0.50946777840000002</v>
       </c>
       <c r="R55">
         <f t="shared" si="2"/>
-        <v>0.99053222159999998</v>
+        <v>0.49053222159999998</v>
       </c>
       <c r="S55" t="b">
         <f t="shared" si="3"/>
@@ -13999,11 +13999,11 @@
       </c>
       <c r="Q56">
         <f t="shared" si="1"/>
-        <v>-1.0017815654666666</v>
+        <v>-0.50178156546666663</v>
       </c>
       <c r="R56">
         <f t="shared" si="2"/>
-        <v>0.99821843453333337</v>
+        <v>0.49821843453333331</v>
       </c>
       <c r="S56" t="b">
         <f t="shared" si="3"/>
@@ -14076,11 +14076,11 @@
       </c>
       <c r="Q57">
         <f t="shared" si="1"/>
-        <v>-0.99911965273333336</v>
+        <v>-0.49911965273333331</v>
       </c>
       <c r="R57">
         <f t="shared" si="2"/>
-        <v>1.0008803472666667</v>
+        <v>0.50088034726666664</v>
       </c>
       <c r="S57" t="b">
         <f t="shared" si="3"/>
@@ -14153,11 +14153,11 @@
       </c>
       <c r="Q58">
         <f t="shared" si="1"/>
-        <v>-0.99649013083333338</v>
+        <v>-0.49649013083333332</v>
       </c>
       <c r="R58">
         <f t="shared" si="2"/>
-        <v>1.0035098691666666</v>
+        <v>0.50350986916666662</v>
       </c>
       <c r="S58" t="b">
         <f t="shared" si="3"/>
@@ -14230,11 +14230,11 @@
       </c>
       <c r="Q59">
         <f t="shared" si="1"/>
-        <v>-0.99447436946666667</v>
+        <v>-0.49447436946666667</v>
       </c>
       <c r="R59">
         <f t="shared" si="2"/>
-        <v>1.0055256305333333</v>
+        <v>0.50552563053333333</v>
       </c>
       <c r="S59" t="b">
         <f t="shared" si="3"/>
@@ -14307,11 +14307,11 @@
       </c>
       <c r="Q60">
         <f t="shared" si="1"/>
-        <v>-0.98544051646666664</v>
+        <v>-0.48544051646666664</v>
       </c>
       <c r="R60">
         <f t="shared" si="2"/>
-        <v>1.0145594835333334</v>
+        <v>0.51455948353333336</v>
       </c>
       <c r="S60" t="b">
         <f t="shared" si="3"/>
@@ -14384,11 +14384,11 @@
       </c>
       <c r="Q61">
         <f t="shared" si="1"/>
-        <v>-0.98388587503333336</v>
+        <v>-0.48388587503333336</v>
       </c>
       <c r="R61">
         <f t="shared" si="2"/>
-        <v>1.0161141249666668</v>
+        <v>0.51611412496666664</v>
       </c>
       <c r="S61" t="b">
         <f t="shared" si="3"/>
@@ -14461,11 +14461,11 @@
       </c>
       <c r="Q62">
         <f t="shared" si="1"/>
-        <v>-0.98146877519999998</v>
+        <v>-0.48146877519999998</v>
       </c>
       <c r="R62">
         <f t="shared" si="2"/>
-        <v>1.0185312248</v>
+        <v>0.51853122480000002</v>
       </c>
       <c r="S62" t="b">
         <f t="shared" si="3"/>
@@ -14538,11 +14538,11 @@
       </c>
       <c r="Q63">
         <f t="shared" si="1"/>
-        <v>-0.97435261279999996</v>
+        <v>-0.47435261280000002</v>
       </c>
       <c r="R63">
         <f t="shared" si="2"/>
-        <v>1.0256473872</v>
+        <v>0.52564738720000004</v>
       </c>
       <c r="S63" t="b">
         <f t="shared" si="3"/>
@@ -14615,11 +14615,11 @@
       </c>
       <c r="Q64">
         <f t="shared" si="1"/>
-        <v>-0.97161072986666663</v>
+        <v>-0.47161072986666669</v>
       </c>
       <c r="R64">
         <f t="shared" si="2"/>
-        <v>1.0283892701333333</v>
+        <v>0.52838927013333337</v>
       </c>
       <c r="S64" t="b">
         <f t="shared" si="3"/>
@@ -14692,11 +14692,11 @@
       </c>
       <c r="Q65">
         <f t="shared" si="1"/>
-        <v>-0.96934669983333333</v>
+        <v>-0.46934669983333333</v>
       </c>
       <c r="R65">
         <f t="shared" si="2"/>
-        <v>1.0306533001666667</v>
+        <v>0.53065330016666667</v>
       </c>
       <c r="S65" t="b">
         <f t="shared" si="3"/>
@@ -14769,11 +14769,11 @@
       </c>
       <c r="Q66">
         <f t="shared" si="1"/>
-        <v>-0.96286784096666667</v>
+        <v>-0.46286784096666667</v>
       </c>
       <c r="R66">
         <f t="shared" si="2"/>
-        <v>1.0371321590333333</v>
+        <v>0.53713215903333333</v>
       </c>
       <c r="S66" t="b">
         <f t="shared" si="3"/>
@@ -14846,14 +14846,14 @@
       </c>
       <c r="Q67">
         <f t="shared" ref="Q67:Q101" si="5">N67-$U$3</f>
-        <v>-0.95377146893333331</v>
+        <v>-0.45377146893333331</v>
       </c>
       <c r="R67">
         <f t="shared" ref="R67:R101" si="6">N67+$U$3</f>
-        <v>1.0462285310666666</v>
+        <v>0.54622853106666669</v>
       </c>
       <c r="S67" t="b">
-        <f t="shared" ref="S67:S101" si="7">OR(O67&lt;Q67,O67&gt;R67)</f>
+        <f t="shared" ref="S67:S101" si="7">OR(AND(O67&lt;Q67,O67&lt;0),AND(O67&gt;R67,O67&gt;0))</f>
         <v>0</v>
       </c>
     </row>
@@ -14923,11 +14923,11 @@
       </c>
       <c r="Q68">
         <f t="shared" si="5"/>
-        <v>-0.94952539250000001</v>
+        <v>-0.44952539250000001</v>
       </c>
       <c r="R68">
         <f t="shared" si="6"/>
-        <v>1.0504746075</v>
+        <v>0.55047460749999999</v>
       </c>
       <c r="S68" t="b">
         <f t="shared" si="7"/>
@@ -15000,11 +15000,11 @@
       </c>
       <c r="Q69">
         <f t="shared" si="5"/>
-        <v>-0.94394067383333335</v>
+        <v>-0.44394067383333335</v>
       </c>
       <c r="R69">
         <f t="shared" si="6"/>
-        <v>1.0560593261666666</v>
+        <v>0.55605932616666665</v>
       </c>
       <c r="S69" t="b">
         <f t="shared" si="7"/>
@@ -15077,11 +15077,11 @@
       </c>
       <c r="Q70">
         <f t="shared" si="5"/>
-        <v>-0.9381346505</v>
+        <v>-0.4381346505</v>
       </c>
       <c r="R70">
         <f t="shared" si="6"/>
-        <v>1.0618653495000001</v>
+        <v>0.5618653495</v>
       </c>
       <c r="S70" t="b">
         <f t="shared" si="7"/>
@@ -15154,11 +15154,11 @@
       </c>
       <c r="Q71">
         <f t="shared" si="5"/>
-        <v>-0.93529985193333331</v>
+        <v>-0.43529985193333331</v>
       </c>
       <c r="R71">
         <f t="shared" si="6"/>
-        <v>1.0647001480666667</v>
+        <v>0.56470014806666669</v>
       </c>
       <c r="S71" t="b">
         <f t="shared" si="7"/>
@@ -15231,11 +15231,11 @@
       </c>
       <c r="Q72">
         <f t="shared" si="5"/>
-        <v>-0.93126309500000004</v>
+        <v>-0.43126309499999999</v>
       </c>
       <c r="R72">
         <f t="shared" si="6"/>
-        <v>1.068736905</v>
+        <v>0.56873690499999996</v>
       </c>
       <c r="S72" t="b">
         <f t="shared" si="7"/>
@@ -15308,11 +15308,11 @@
       </c>
       <c r="Q73">
         <f t="shared" si="5"/>
-        <v>-0.92385755280000004</v>
+        <v>-0.42385755279999998</v>
       </c>
       <c r="R73">
         <f t="shared" si="6"/>
-        <v>1.0761424472000001</v>
+        <v>0.57614244719999996</v>
       </c>
       <c r="S73" t="b">
         <f t="shared" si="7"/>
@@ -15385,11 +15385,11 @@
       </c>
       <c r="Q74">
         <f t="shared" si="5"/>
-        <v>-0.91095381796666663</v>
+        <v>-0.41095381796666669</v>
       </c>
       <c r="R74">
         <f t="shared" si="6"/>
-        <v>1.0890461820333333</v>
+        <v>0.58904618203333337</v>
       </c>
       <c r="S74" t="b">
         <f t="shared" si="7"/>
@@ -15462,11 +15462,11 @@
       </c>
       <c r="Q75">
         <f t="shared" si="5"/>
-        <v>-0.9095589405333333</v>
+        <v>-0.4095589405333333</v>
       </c>
       <c r="R75">
         <f t="shared" si="6"/>
-        <v>1.0904410594666667</v>
+        <v>0.5904410594666667</v>
       </c>
       <c r="S75" t="b">
         <f t="shared" si="7"/>
@@ -15539,11 +15539,11 @@
       </c>
       <c r="Q76">
         <f t="shared" si="5"/>
-        <v>-0.90179353920000005</v>
+        <v>-0.40179353919999999</v>
       </c>
       <c r="R76">
         <f t="shared" si="6"/>
-        <v>1.0982064608</v>
+        <v>0.59820646079999995</v>
       </c>
       <c r="S76" t="b">
         <f t="shared" si="7"/>
@@ -15616,11 +15616,11 @@
       </c>
       <c r="Q77">
         <f t="shared" si="5"/>
-        <v>-0.88301834089999998</v>
+        <v>-0.38301834090000003</v>
       </c>
       <c r="R77">
         <f t="shared" si="6"/>
-        <v>1.1169816590999999</v>
+        <v>0.61698165910000002</v>
       </c>
       <c r="S77" t="b">
         <f t="shared" si="7"/>
@@ -15693,11 +15693,11 @@
       </c>
       <c r="Q78">
         <f t="shared" si="5"/>
-        <v>-0.87813437626666668</v>
+        <v>-0.37813437626666668</v>
       </c>
       <c r="R78">
         <f t="shared" si="6"/>
-        <v>1.1218656237333333</v>
+        <v>0.62186562373333332</v>
       </c>
       <c r="S78" t="b">
         <f t="shared" si="7"/>
@@ -15770,11 +15770,11 @@
       </c>
       <c r="Q79">
         <f t="shared" si="5"/>
-        <v>-0.84922670950000001</v>
+        <v>-0.34922670950000001</v>
       </c>
       <c r="R79">
         <f t="shared" si="6"/>
-        <v>1.1507732905000001</v>
+        <v>0.65077329049999999</v>
       </c>
       <c r="S79" t="b">
         <f t="shared" si="7"/>
@@ -15847,11 +15847,11 @@
       </c>
       <c r="Q80">
         <f t="shared" si="5"/>
-        <v>-0.84281695593333339</v>
+        <v>-0.34281695593333339</v>
       </c>
       <c r="R80">
         <f t="shared" si="6"/>
-        <v>1.1571830440666666</v>
+        <v>0.65718304406666661</v>
       </c>
       <c r="S80" t="b">
         <f t="shared" si="7"/>
@@ -15924,11 +15924,11 @@
       </c>
       <c r="Q81">
         <f t="shared" si="5"/>
-        <v>-0.83321944203333331</v>
+        <v>-0.33321944203333331</v>
       </c>
       <c r="R81">
         <f t="shared" si="6"/>
-        <v>1.1667805579666668</v>
+        <v>0.66678055796666669</v>
       </c>
       <c r="S81" t="b">
         <f t="shared" si="7"/>
@@ -16001,11 +16001,11 @@
       </c>
       <c r="Q82">
         <f t="shared" si="5"/>
-        <v>-0.82034347876666669</v>
+        <v>-0.32034347876666669</v>
       </c>
       <c r="R82">
         <f t="shared" si="6"/>
-        <v>1.1796565212333334</v>
+        <v>0.67965652123333331</v>
       </c>
       <c r="S82" t="b">
         <f t="shared" si="7"/>
@@ -16078,11 +16078,11 @@
       </c>
       <c r="Q83">
         <f t="shared" si="5"/>
-        <v>-0.8097037789</v>
+        <v>-0.3097037789</v>
       </c>
       <c r="R83">
         <f t="shared" si="6"/>
-        <v>1.1902962211000001</v>
+        <v>0.6902962211</v>
       </c>
       <c r="S83" t="b">
         <f t="shared" si="7"/>
@@ -16155,11 +16155,11 @@
       </c>
       <c r="Q84">
         <f t="shared" si="5"/>
-        <v>-0.80568685829999998</v>
+        <v>-0.30568685829999998</v>
       </c>
       <c r="R84">
         <f t="shared" si="6"/>
-        <v>1.1943131416999999</v>
+        <v>0.69431314170000002</v>
       </c>
       <c r="S84" t="b">
         <f t="shared" si="7"/>
@@ -16232,11 +16232,11 @@
       </c>
       <c r="Q85">
         <f t="shared" si="5"/>
-        <v>-0.77556074563333333</v>
+        <v>-0.27556074563333333</v>
       </c>
       <c r="R85">
         <f t="shared" si="6"/>
-        <v>1.2244392543666667</v>
+        <v>0.72443925436666667</v>
       </c>
       <c r="S85" t="b">
         <f t="shared" si="7"/>
@@ -16309,11 +16309,11 @@
       </c>
       <c r="Q86">
         <f t="shared" si="5"/>
-        <v>-0.77023242459999997</v>
+        <v>-0.27023242459999997</v>
       </c>
       <c r="R86">
         <f t="shared" si="6"/>
-        <v>1.2297675753999999</v>
+        <v>0.72976757540000003</v>
       </c>
       <c r="S86" t="b">
         <f t="shared" si="7"/>
@@ -16386,11 +16386,11 @@
       </c>
       <c r="Q87">
         <f t="shared" si="5"/>
-        <v>-0.75671930036666668</v>
+        <v>-0.25671930036666668</v>
       </c>
       <c r="R87">
         <f t="shared" si="6"/>
-        <v>1.2432806996333334</v>
+        <v>0.74328069963333332</v>
       </c>
       <c r="S87" t="b">
         <f t="shared" si="7"/>
@@ -16463,11 +16463,11 @@
       </c>
       <c r="Q88">
         <f t="shared" si="5"/>
-        <v>-0.7389294877</v>
+        <v>-0.2389294877</v>
       </c>
       <c r="R88">
         <f t="shared" si="6"/>
-        <v>1.2610705122999999</v>
+        <v>0.7610705123</v>
       </c>
       <c r="S88" t="b">
         <f t="shared" si="7"/>
@@ -16540,11 +16540,11 @@
       </c>
       <c r="Q89">
         <f t="shared" si="5"/>
-        <v>-0.71465507346666668</v>
+        <v>-0.21465507346666668</v>
       </c>
       <c r="R89">
         <f t="shared" si="6"/>
-        <v>1.2853449265333334</v>
+        <v>0.78534492653333332</v>
       </c>
       <c r="S89" t="b">
         <f t="shared" si="7"/>
@@ -16617,11 +16617,11 @@
       </c>
       <c r="Q90">
         <f t="shared" si="5"/>
-        <v>-0.70191987736666661</v>
+        <v>-0.20191987736666667</v>
       </c>
       <c r="R90">
         <f t="shared" si="6"/>
-        <v>1.2980801226333334</v>
+        <v>0.79808012263333339</v>
       </c>
       <c r="S90" t="b">
         <f t="shared" si="7"/>
@@ -16694,11 +16694,11 @@
       </c>
       <c r="Q91">
         <f t="shared" si="5"/>
-        <v>-0.68956877203333333</v>
+        <v>-0.18956877203333333</v>
       </c>
       <c r="R91">
         <f t="shared" si="6"/>
-        <v>1.3104312279666668</v>
+        <v>0.81043122796666667</v>
       </c>
       <c r="S91" t="b">
         <f t="shared" si="7"/>
@@ -16771,11 +16771,11 @@
       </c>
       <c r="Q92">
         <f t="shared" si="5"/>
-        <v>-0.68483942523333341</v>
+        <v>-0.18483942523333335</v>
       </c>
       <c r="R92">
         <f t="shared" si="6"/>
-        <v>1.3151605747666666</v>
+        <v>0.81516057476666659</v>
       </c>
       <c r="S92" t="b">
         <f t="shared" si="7"/>
@@ -16848,11 +16848,11 @@
       </c>
       <c r="Q93">
         <f t="shared" si="5"/>
-        <v>-0.67238517929999997</v>
+        <v>-0.17238517930000002</v>
       </c>
       <c r="R93">
         <f t="shared" si="6"/>
-        <v>1.3276148207</v>
+        <v>0.82761482070000003</v>
       </c>
       <c r="S93" t="b">
         <f t="shared" si="7"/>
@@ -16925,11 +16925,11 @@
       </c>
       <c r="Q94">
         <f t="shared" si="5"/>
-        <v>-0.66079070903333337</v>
+        <v>-0.16079070903333337</v>
       </c>
       <c r="R94">
         <f t="shared" si="6"/>
-        <v>1.3392092909666666</v>
+        <v>0.83920929096666663</v>
       </c>
       <c r="S94" t="b">
         <f t="shared" si="7"/>
@@ -17002,11 +17002,11 @@
       </c>
       <c r="Q95">
         <f t="shared" si="5"/>
-        <v>-0.65706933973333337</v>
+        <v>-0.15706933973333337</v>
       </c>
       <c r="R95">
         <f t="shared" si="6"/>
-        <v>1.3429306602666666</v>
+        <v>0.84293066026666663</v>
       </c>
       <c r="S95" t="b">
         <f t="shared" si="7"/>
@@ -17079,11 +17079,11 @@
       </c>
       <c r="Q96">
         <f t="shared" si="5"/>
-        <v>-0.6019124262333333</v>
+        <v>-0.10191242623333335</v>
       </c>
       <c r="R96">
         <f t="shared" si="6"/>
-        <v>1.3980875737666667</v>
+        <v>0.8980875737666667</v>
       </c>
       <c r="S96" t="b">
         <f t="shared" si="7"/>
@@ -17156,11 +17156,11 @@
       </c>
       <c r="Q97">
         <f t="shared" si="5"/>
-        <v>-0.5393979284999999</v>
+        <v>-3.9397928499999957E-2</v>
       </c>
       <c r="R97">
         <f t="shared" si="6"/>
-        <v>1.4606020715000001</v>
+        <v>0.9606020715000001</v>
       </c>
       <c r="S97" t="b">
         <f t="shared" si="7"/>
@@ -17233,11 +17233,11 @@
       </c>
       <c r="Q98">
         <f t="shared" si="5"/>
-        <v>-0.52216119270000005</v>
+        <v>-2.2161192699999999E-2</v>
       </c>
       <c r="R98">
         <f t="shared" si="6"/>
-        <v>1.4778388072999999</v>
+        <v>0.97783880729999995</v>
       </c>
       <c r="S98" t="b">
         <f t="shared" si="7"/>
@@ -17310,11 +17310,11 @@
       </c>
       <c r="Q99">
         <f t="shared" si="5"/>
-        <v>-0.44245440973333328</v>
+        <v>5.7545590266666724E-2</v>
       </c>
       <c r="R99">
         <f t="shared" si="6"/>
-        <v>1.5575455902666668</v>
+        <v>1.0575455902666668</v>
       </c>
       <c r="S99" t="b">
         <f t="shared" si="7"/>
@@ -17387,11 +17387,11 @@
       </c>
       <c r="Q100">
         <f t="shared" si="5"/>
-        <v>-0.17865609999999998</v>
+        <v>0.32134390000000002</v>
       </c>
       <c r="R100">
         <f t="shared" si="6"/>
-        <v>1.8213439</v>
+        <v>1.3213439</v>
       </c>
       <c r="S100" t="b">
         <f t="shared" si="7"/>
@@ -17464,11 +17464,11 @@
       </c>
       <c r="Q101">
         <f t="shared" si="5"/>
-        <v>0.1680629543333334</v>
+        <v>0.6680629543333334</v>
       </c>
       <c r="R101">
         <f t="shared" si="6"/>
-        <v>2.1680629543333332</v>
+        <v>1.6680629543333334</v>
       </c>
       <c r="S101" t="b">
         <f t="shared" si="7"/>

</xml_diff>